<commit_message>
Chatbot with 2 knn models for classif.
</commit_message>
<xml_diff>
--- a/batch.xlsx
+++ b/batch.xlsx
@@ -12,8 +12,9 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="9510" windowHeight="3150"/>
   </bookViews>
   <sheets>
-    <sheet name="Mensajes" sheetId="2" r:id="rId1"/>
-    <sheet name="Dicc." sheetId="1" r:id="rId2"/>
+    <sheet name="Tranning_knn_1" sheetId="6" r:id="rId1"/>
+    <sheet name="Trainning_knn_2" sheetId="2" r:id="rId2"/>
+    <sheet name="Diccionary" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
   <si>
     <t>Palabras</t>
   </si>
@@ -57,30 +58,9 @@
     <t>retraso</t>
   </si>
   <si>
-    <t>Quiero los tickets de la semana</t>
-  </si>
-  <si>
-    <t>Tuve un retraso con un ticket</t>
-  </si>
-  <si>
     <t>MENSAJE</t>
   </si>
   <si>
-    <t>Hola, necesito informacion de un ticket</t>
-  </si>
-  <si>
-    <t>Necesito informacion de un tecnico que me atendio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hoy tuve un problema con un tecnico </t>
-  </si>
-  <si>
-    <t>Tengo un numero de atencion</t>
-  </si>
-  <si>
-    <t>Necesito la informacion de un ticket por un problema</t>
-  </si>
-  <si>
     <t>atencion</t>
   </si>
   <si>
@@ -109,6 +89,60 @@
   </si>
   <si>
     <t>un tecnico no soluciono el ticket que envie</t>
+  </si>
+  <si>
+    <t>W1</t>
+  </si>
+  <si>
+    <t>W2</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>hola</t>
+  </si>
+  <si>
+    <t>como</t>
+  </si>
+  <si>
+    <t>buenos</t>
+  </si>
+  <si>
+    <t>tuve un retraso con un ticket</t>
+  </si>
+  <si>
+    <t>necesito la informacion de un ticket por un problema</t>
+  </si>
+  <si>
+    <t>tengo un numero de atencion</t>
+  </si>
+  <si>
+    <t>quiero los tickets de la semana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hoy tuve un problema con un tecnico </t>
+  </si>
+  <si>
+    <t>necesito informacion de un tecnico que me atendio</t>
+  </si>
+  <si>
+    <t>hola, necesito informacion de un ticket</t>
+  </si>
+  <si>
+    <t>hola tengo un problema</t>
+  </si>
+  <si>
+    <t>buenos dias</t>
+  </si>
+  <si>
+    <t>necestio informacion</t>
+  </si>
+  <si>
+    <t>hola como estas</t>
+  </si>
+  <si>
+    <t>no tengo el numero de ticket</t>
   </si>
 </sst>
 </file>
@@ -144,9 +178,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,10 +465,197 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="49" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>12345</v>
+      </c>
+      <c r="B7" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>32165</v>
+      </c>
+      <c r="B8" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>14564</v>
+      </c>
+      <c r="B9" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,15 +668,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -459,7 +684,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -467,7 +692,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -475,7 +700,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -483,7 +708,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -491,7 +716,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -499,7 +724,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -507,7 +732,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -515,7 +740,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -523,7 +748,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -531,7 +756,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B12" s="1">
         <v>2</v>
@@ -539,7 +764,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B13" s="1">
         <v>2</v>
@@ -551,12 +776,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,7 +789,7 @@
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -574,8 +799,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -585,10 +816,16 @@
       <c r="C2">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>0.6</v>
@@ -596,10 +833,16 @@
       <c r="C3">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>0.1</v>
@@ -607,10 +850,16 @@
       <c r="C4">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>0.3</v>
@@ -618,8 +867,14 @@
       <c r="C5">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -629,8 +884,14 @@
       <c r="C6">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -640,8 +901,14 @@
       <c r="C7">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -651,10 +918,16 @@
       <c r="C8">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B9">
         <v>0.5</v>
@@ -662,8 +935,14 @@
       <c r="C9">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -673,8 +952,14 @@
       <c r="C10">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -684,8 +969,14 @@
       <c r="C11">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -695,10 +986,16 @@
       <c r="C12">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B13">
         <v>0.1</v>
@@ -706,8 +1003,83 @@
       <c r="C13">
         <v>0.9</v>
       </c>
+      <c r="D13" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14">
+        <v>0.5</v>
+      </c>
+      <c r="C14">
+        <v>0.5</v>
+      </c>
+      <c r="D14">
+        <v>0.1</v>
+      </c>
+      <c r="E14">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15">
+        <v>0.5</v>
+      </c>
+      <c r="C15">
+        <v>0.5</v>
+      </c>
+      <c r="D15">
+        <v>0.3</v>
+      </c>
+      <c r="E15">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16">
+        <v>0.5</v>
+      </c>
+      <c r="C16">
+        <v>0.5</v>
+      </c>
+      <c r="D16">
+        <v>0.3</v>
+      </c>
+      <c r="E16">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17">
+        <v>0.5</v>
+      </c>
+      <c r="C17">
+        <v>0.5</v>
+      </c>
+      <c r="D17">
+        <v>0.3</v>
+      </c>
+      <c r="E17">
+        <v>0.7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>